<commit_message>
Update on SamsaraUITest, updating locator for nextButton
</commit_message>
<xml_diff>
--- a/Red vs Samsara.xlsx
+++ b/Red vs Samsara.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>Bugs</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Logout button on landing page</t>
+  </si>
+  <si>
+    <t>Next page button is hard to get due to font</t>
   </si>
 </sst>
 </file>
@@ -845,10 +848,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,6 +881,11 @@
         <v>42</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates on samsara ui tests
</commit_message>
<xml_diff>
--- a/Red vs Samsara.xlsx
+++ b/Red vs Samsara.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="159" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="159" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
-    <sheet name="Bugs" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Bugs" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Bugs</t>
   </si>
@@ -135,9 +136,6 @@
 2. On Login Page enter invalid credentials in username field
 3. On Login page, click Log in button
 Expected: Login denied. Error message "Invalid username and password." displayed</t>
-  </si>
-  <si>
-    <t>userCreateNewHeroTest</t>
   </si>
   <si>
     <t>userEditExistingOwnHeroTest</t>
@@ -180,6 +178,54 @@
   </si>
   <si>
     <t>Next page button is hard to get due to font</t>
+  </si>
+  <si>
+    <t>testCreateNewHeroAsUser</t>
+  </si>
+  <si>
+    <t>Test steps</t>
+  </si>
+  <si>
+    <t>[INFO] Tests run: 45, Failures: 0, Errors: 0, Skipped: 0, Time elapsed: 249.082 s - in TestSuite</t>
+  </si>
+  <si>
+    <t>[INFO]</t>
+  </si>
+  <si>
+    <t>[INFO] Results:</t>
+  </si>
+  <si>
+    <t>[INFO] Tests run: 45, Failures: 0, Errors: 0, Skipped: 0</t>
+  </si>
+  <si>
+    <t>[WARNING] File encoding has not been set, using platform encoding Cp1252, i.e. build is platform dependent! The file encoding for reports output files should be provided by the POM property ${project.reporting.outputEncoding}.</t>
+  </si>
+  <si>
+    <t>[INFO] --- maven-failsafe-plugin:2.20:verify (default) @ RedTestFramework ---</t>
+  </si>
+  <si>
+    <t>[INFO] --- maven-install-plugin:2.4:install (default-install) @ RedTestFramework ---</t>
+  </si>
+  <si>
+    <t>[INFO] Installing C:\Users\Marko\Documents\Automation\RED\RedTestFramework\target\RedTestFramework-0.0.1-SNAPSHOT.jar to C:\Users\Marko\.m2\repository\com\red\testframework\RedTestFramework\0.0.1-SNAPSHOT\RedTestFramework-0.0.1-SNAPSHOT.jar</t>
+  </si>
+  <si>
+    <t>[INFO] Installing C:\Users\Marko\Documents\Automation\RED\RedTestFramework\pom.xml to C:\Users\Marko\.m2\repository\com\red\testframework\RedTestFramework\0.0.1-SNAPSHOT\RedTestFramework-0.0.1-SNAPSHOT.pom</t>
+  </si>
+  <si>
+    <t>[INFO] ------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>[INFO] BUILD SUCCESS</t>
+  </si>
+  <si>
+    <t>[INFO] Total time: 04:15 min</t>
+  </si>
+  <si>
+    <t>[INFO] Finished at: 2020-05-03T21:46:26+02:00</t>
+  </si>
+  <si>
+    <t>[INFO] Final Memory: 25M/416M</t>
   </si>
 </sst>
 </file>
@@ -250,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -269,6 +315,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,25 +605,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="81.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="223.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="81.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="223.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -579,268 +635,359 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="180" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="B12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="B13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="F13" s="5"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="F14" s="5"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="F15" s="5"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="3"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G27" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B4:B11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -848,9 +995,132 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="247" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9">
+        <v>43954</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -863,27 +1133,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>